<commit_message>
Power comparisons for 3x2.
</commit_message>
<xml_diff>
--- a/power_comp_1_row_10_10_col_2.xlsx
+++ b/power_comp_1_row_10_10_col_2.xlsx
@@ -71,10 +71,10 @@
     <t xml:space="preserve">&lt; -0.0679</t>
   </si>
   <si>
-    <t xml:space="preserve">0.6632 0.0184</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.3364 -0.0184</t>
+    <t xml:space="preserve">0.66 0.0184</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.3398 -0.0184</t>
   </si>
 </sst>
 </file>

</xml_diff>